<commit_message>
Finish Envi data cleaning
Created a new folder for final envi data for analysis
</commit_message>
<xml_diff>
--- a/2012_EPA/raw/Solar_Cord_book.xlsx
+++ b/2012_EPA/raw/Solar_Cord_book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\OmniBEF_NLA\NLA_Data\2012_EPA\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A0C379BD-08D5-4C7F-9030-29F5175D42CC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4FD46745-9C8E-4C53-85C1-9561B5DF8329}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{6AA70A5E-7DA2-4A5C-9F1F-ED5132B237F7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="2">
   <si>
     <t>v</t>
   </si>
@@ -382,15 +382,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B7D0B0-8568-40CB-A944-E75AB1FC92FE}">
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87:E88"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E82" sqref="E82:F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>26</v>
       </c>
@@ -408,8 +408,11 @@
       <c r="E1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>A1+4</f>
         <v>30</v>
@@ -422,14 +425,17 @@
         <v>34</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D7" si="1">B2+4</f>
+        <f t="shared" ref="D2:D6" si="1">B2+4</f>
         <v>-120.25</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+4</f>
         <v>34</v>
@@ -448,10 +454,13 @@
       <c r="E3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A7" si="2">A3+4</f>
+        <f t="shared" ref="A4:A6" si="2">A3+4</f>
         <v>38</v>
       </c>
       <c r="B4">
@@ -468,8 +477,11 @@
       <c r="E4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -488,8 +500,11 @@
       <c r="E5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -508,8 +523,11 @@
       <c r="E6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>26</v>
       </c>
@@ -521,14 +539,17 @@
         <v>30</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:D13" si="4">B7+4</f>
+        <f t="shared" ref="D7:D12" si="4">B7+4</f>
         <v>-116.25</v>
       </c>
       <c r="E7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>A7+4</f>
         <v>30</v>
@@ -547,8 +568,11 @@
       <c r="E8" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>A8+4</f>
         <v>34</v>
@@ -567,8 +591,11 @@
       <c r="E9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ref="A10:A12" si="5">A9+4</f>
         <v>38</v>
@@ -587,8 +614,11 @@
       <c r="E10" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="5"/>
         <v>42</v>
@@ -607,8 +637,11 @@
       <c r="E11" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="5"/>
         <v>46</v>
@@ -627,8 +660,11 @@
       <c r="E12" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>26</v>
       </c>
@@ -646,8 +682,11 @@
       <c r="E13" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>A13+4</f>
         <v>30</v>
@@ -666,8 +705,11 @@
       <c r="E14" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <f>A14+4</f>
         <v>34</v>
@@ -686,8 +728,11 @@
       <c r="E15" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ref="A16:A18" si="8">A15+4</f>
         <v>38</v>
@@ -706,8 +751,11 @@
       <c r="E16" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="8"/>
         <v>42</v>
@@ -726,8 +774,11 @@
       <c r="E17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="8"/>
         <v>46</v>
@@ -746,8 +797,11 @@
       <c r="E18" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>26</v>
       </c>
@@ -765,8 +819,11 @@
       <c r="E19" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <f>A19+4</f>
         <v>30</v>
@@ -785,8 +842,11 @@
       <c r="E20" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <f>A20+4</f>
         <v>34</v>
@@ -805,8 +865,11 @@
       <c r="E21" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" ref="A22:A24" si="9">A21+4</f>
         <v>38</v>
@@ -825,8 +888,11 @@
       <c r="E22" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="9"/>
         <v>42</v>
@@ -845,8 +911,11 @@
       <c r="E23" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="9"/>
         <v>46</v>
@@ -865,8 +934,11 @@
       <c r="E24" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>26</v>
       </c>
@@ -884,8 +956,11 @@
       <c r="E25" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <f>A25+4</f>
         <v>30</v>
@@ -904,8 +979,11 @@
       <c r="E26" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <f>A26+4</f>
         <v>34</v>
@@ -924,8 +1002,11 @@
       <c r="E27" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" ref="A28:A30" si="10">A27+4</f>
         <v>38</v>
@@ -944,8 +1025,11 @@
       <c r="E28" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="10"/>
         <v>42</v>
@@ -964,8 +1048,11 @@
       <c r="E29" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="10"/>
         <v>46</v>
@@ -984,8 +1071,11 @@
       <c r="E30" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>26</v>
       </c>
@@ -1003,8 +1093,11 @@
       <c r="E31" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <f>A31+4</f>
         <v>30</v>
@@ -1023,8 +1116,11 @@
       <c r="E32" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <f>A32+4</f>
         <v>34</v>
@@ -1043,8 +1139,11 @@
       <c r="E33" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" ref="A34:A36" si="11">A33+4</f>
         <v>38</v>
@@ -1063,8 +1162,11 @@
       <c r="E34" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="11"/>
         <v>42</v>
@@ -1083,8 +1185,11 @@
       <c r="E35" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="11"/>
         <v>46</v>
@@ -1103,8 +1208,11 @@
       <c r="E36" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>26</v>
       </c>
@@ -1122,8 +1230,11 @@
       <c r="E37" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <f>A37+4</f>
         <v>30</v>
@@ -1142,8 +1253,11 @@
       <c r="E38" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <f>A38+4</f>
         <v>34</v>
@@ -1152,18 +1266,21 @@
         <v>-100.25</v>
       </c>
       <c r="C39">
-        <f t="shared" ref="C39:C96" si="12">A39+4</f>
+        <f t="shared" ref="C39:C90" si="12">A39+4</f>
         <v>38</v>
       </c>
       <c r="D39">
-        <f t="shared" ref="D39:D96" si="13">B39+4</f>
+        <f t="shared" ref="D39:D90" si="13">B39+4</f>
         <v>-96.25</v>
       </c>
       <c r="E39" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" ref="A40:A42" si="14">A39+4</f>
         <v>38</v>
@@ -1182,8 +1299,11 @@
       <c r="E40" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="14"/>
         <v>42</v>
@@ -1202,8 +1322,11 @@
       <c r="E41" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="14"/>
         <v>46</v>
@@ -1222,8 +1345,11 @@
       <c r="E42" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>26</v>
       </c>
@@ -1241,8 +1367,11 @@
       <c r="E43" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <f>A43+4</f>
         <v>30</v>
@@ -1261,8 +1390,11 @@
       <c r="E44" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <f>A44+4</f>
         <v>34</v>
@@ -1281,8 +1413,11 @@
       <c r="E45" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" ref="A46:A48" si="15">A45+4</f>
         <v>38</v>
@@ -1301,8 +1436,11 @@
       <c r="E46" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="15"/>
         <v>42</v>
@@ -1321,8 +1459,11 @@
       <c r="E47" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="15"/>
         <v>46</v>
@@ -1341,8 +1482,11 @@
       <c r="E48" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>26</v>
       </c>
@@ -1360,8 +1504,11 @@
       <c r="E49" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <f>A49+4</f>
         <v>30</v>
@@ -1380,8 +1527,11 @@
       <c r="E50" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <f>A50+4</f>
         <v>34</v>
@@ -1400,8 +1550,11 @@
       <c r="E51" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" ref="A52:A54" si="16">A51+4</f>
         <v>38</v>
@@ -1420,8 +1573,11 @@
       <c r="E52" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="16"/>
         <v>42</v>
@@ -1440,8 +1596,11 @@
       <c r="E53" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="16"/>
         <v>46</v>
@@ -1460,8 +1619,11 @@
       <c r="E54" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>26</v>
       </c>
@@ -1479,8 +1641,11 @@
       <c r="E55" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <f>A55+4</f>
         <v>30</v>
@@ -1499,8 +1664,11 @@
       <c r="E56" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <f>A56+4</f>
         <v>34</v>
@@ -1519,8 +1687,11 @@
       <c r="E57" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" ref="A58:A60" si="17">A57+4</f>
         <v>38</v>
@@ -1539,8 +1710,11 @@
       <c r="E58" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="17"/>
         <v>42</v>
@@ -1559,8 +1733,11 @@
       <c r="E59" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="17"/>
         <v>46</v>
@@ -1579,8 +1756,11 @@
       <c r="E60" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>26</v>
       </c>
@@ -1598,8 +1778,11 @@
       <c r="E61" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <f>A61+4</f>
         <v>30</v>
@@ -1618,8 +1801,11 @@
       <c r="E62" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <f>A62+4</f>
         <v>34</v>
@@ -1638,8 +1824,11 @@
       <c r="E63" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" ref="A64:A66" si="18">A63+4</f>
         <v>38</v>
@@ -1658,8 +1847,11 @@
       <c r="E64" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="18"/>
         <v>42</v>
@@ -1678,8 +1870,11 @@
       <c r="E65" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="18"/>
         <v>46</v>
@@ -1698,8 +1893,11 @@
       <c r="E66" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>26</v>
       </c>
@@ -1717,8 +1915,11 @@
       <c r="E67" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <f>A67+4</f>
         <v>30</v>
@@ -1737,8 +1938,11 @@
       <c r="E68" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <f>A68+4</f>
         <v>34</v>
@@ -1757,8 +1961,11 @@
       <c r="E69" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" ref="A70:A72" si="19">A69+4</f>
         <v>38</v>
@@ -1777,8 +1984,11 @@
       <c r="E70" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" si="19"/>
         <v>42</v>
@@ -1797,8 +2007,11 @@
       <c r="E71" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" si="19"/>
         <v>46</v>
@@ -1817,8 +2030,11 @@
       <c r="E72" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>26</v>
       </c>
@@ -1836,8 +2052,11 @@
       <c r="E73" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <f>A73+4</f>
         <v>30</v>
@@ -1856,8 +2075,11 @@
       <c r="E74" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <f>A74+4</f>
         <v>34</v>
@@ -1876,8 +2098,11 @@
       <c r="E75" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <f t="shared" ref="A76:A78" si="20">A75+4</f>
         <v>38</v>
@@ -1896,8 +2121,11 @@
       <c r="E76" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <f t="shared" si="20"/>
         <v>42</v>
@@ -1916,8 +2144,11 @@
       <c r="E77" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <f t="shared" si="20"/>
         <v>46</v>
@@ -1936,8 +2167,11 @@
       <c r="E78" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F78" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>26</v>
       </c>
@@ -1955,8 +2189,11 @@
       <c r="E79" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <f>A79+4</f>
         <v>30</v>
@@ -1975,8 +2212,11 @@
       <c r="E80" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F80" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <f>A80+4</f>
         <v>34</v>
@@ -1995,8 +2235,11 @@
       <c r="E81" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F81" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <f t="shared" ref="A82:A84" si="21">A81+4</f>
         <v>38</v>
@@ -2015,8 +2258,11 @@
       <c r="E82" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F82" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="21"/>
         <v>42</v>
@@ -2035,8 +2281,11 @@
       <c r="E83" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F83" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" si="21"/>
         <v>46</v>
@@ -2055,8 +2304,11 @@
       <c r="E84" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F84" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>26</v>
       </c>
@@ -2074,8 +2326,11 @@
       <c r="E85" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F85" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <f>A85+4</f>
         <v>30</v>
@@ -2094,8 +2349,11 @@
       <c r="E86" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F86" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <f>A86+4</f>
         <v>34</v>
@@ -2114,8 +2372,11 @@
       <c r="E87" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F87" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" ref="A88:A90" si="22">A87+4</f>
         <v>38</v>
@@ -2134,8 +2395,11 @@
       <c r="E88" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F88" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" si="22"/>
         <v>42</v>
@@ -2154,8 +2418,11 @@
       <c r="E89" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F89" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <f t="shared" si="22"/>
         <v>46</v>
@@ -2172,6 +2439,9 @@
         <v>-64.25</v>
       </c>
       <c r="E90" t="s">
+        <v>0</v>
+      </c>
+      <c r="F90" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>